<commit_message>
Update spreadsheets: fix incorrect url in example and change headers to match interface
</commit_message>
<xml_diff>
--- a/dashboard/internet_nl_dashboard/static/sample_spreadsheets/microsoft_office_spreadsheet_with_example_data.xlsx
+++ b/dashboard/internet_nl_dashboard/static/sample_spreadsheets/microsoft_office_spreadsheet_with_example_data.xlsx
@@ -8,11 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Internet Addresses" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Statistics" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Domains" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="data" vbProcedure="false">'Internet Addresses'!$A:$B</definedName>
+    <definedName function="false" hidden="false" name="data" vbProcedure="false">Domains!$A:$B</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
-  <si>
-    <t xml:space="preserve">Category / List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internet Address</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain</t>
   </si>
   <si>
     <t xml:space="preserve">waterschappen, testsites</t>
@@ -83,7 +82,7 @@
     <t xml:space="preserve">scheldestromen.nl</t>
   </si>
   <si>
-    <t xml:space="preserve">schielandenkrimenerwaard.nl</t>
+    <t xml:space="preserve">schielandendekrimpenerwaard.nl</t>
   </si>
   <si>
     <t xml:space="preserve">hdsr.nl</t>
@@ -102,18 +101,6 @@
   </si>
   <si>
     <t xml:space="preserve">zuiderzeeland.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To Reload: right click the table and choose “refresh”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count - Internet Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(empty)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Result</t>
   </si>
 </sst>
 </file>
@@ -129,6 +116,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,6 +132,65 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -151,82 +198,36 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -235,6 +236,42 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -242,44 +279,8 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -302,69 +303,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -390,40 +328,82 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,54 +412,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="37" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="39" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="39" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="37" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="40" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="38" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="40" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="38" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="38" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="9" xfId="41" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="42" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -491,29 +423,29 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
-    <cellStyle name="Pivot Table Corner" xfId="37"/>
-    <cellStyle name="Pivot Table Value" xfId="38"/>
-    <cellStyle name="Pivot Table Field" xfId="39"/>
-    <cellStyle name="Pivot Table Category" xfId="40"/>
-    <cellStyle name="Pivot Table Title" xfId="41"/>
-    <cellStyle name="Pivot Table Result" xfId="42"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Pivot Table Category" xfId="34"/>
+    <cellStyle name="Pivot Table Corner" xfId="35"/>
+    <cellStyle name="Pivot Table Field" xfId="36"/>
+    <cellStyle name="Pivot Table Result" xfId="37"/>
+    <cellStyle name="Pivot Table Title" xfId="38"/>
+    <cellStyle name="Pivot Table Value" xfId="39"/>
+    <cellStyle name="Status 10" xfId="40"/>
+    <cellStyle name="Text 6" xfId="41"/>
+    <cellStyle name="Warning 14" xfId="42"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -583,7 +515,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -594,7 +526,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -790,9 +722,6 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -803,83 +732,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="15" t="n">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>